<commit_message>
Added Tags, Pattern and Respones
</commit_message>
<xml_diff>
--- a/intent_ergänzungen.xlsx
+++ b/intent_ergänzungen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI_Unterlagen\ChatBot_Projekt\Chatbot\chatbot_intents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabian\Git_Projekte\chatbots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C3B859-8460-467A-9C9A-83DC5C35E69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DAE7FE-1E6A-4622-8539-F6757AA516BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{013106A1-32B2-4123-9546-0C6B8C3BE0C4}"/>
   </bookViews>
@@ -185,12 +185,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -205,9 +217,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -525,7 +539,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,157 +565,176 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="D16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new content, tags and patterns
</commit_message>
<xml_diff>
--- a/intent_ergänzungen.xlsx
+++ b/intent_ergänzungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabia\Git_Projekte\chatbots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Laura/Desktop/chatbots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C960376-CAF0-43AE-94B2-496BBBF6C718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F73D1AE-C3B0-DB4D-8B47-5865DCB507BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{013106A1-32B2-4123-9546-0C6B8C3BE0C4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{013106A1-32B2-4123-9546-0C6B8C3BE0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Tag to add</t>
   </si>
@@ -164,6 +164,39 @@
   </si>
   <si>
     <t xml:space="preserve">i dont like that </t>
+  </si>
+  <si>
+    <t>medizinkram pattern erweitert</t>
+  </si>
+  <si>
+    <t>hungry</t>
+  </si>
+  <si>
+    <t>i am hungry…</t>
+  </si>
+  <si>
+    <t>i am also hungry</t>
+  </si>
+  <si>
+    <t>like_simple</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> falls wir like noch brauchen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i like football </t>
+  </si>
+  <si>
+    <t>That is very nice, tell me more</t>
+  </si>
+  <si>
+    <t>dontLike</t>
+  </si>
+  <si>
+    <t>I don't like football</t>
+  </si>
+  <si>
+    <t>I agree with you</t>
   </si>
 </sst>
 </file>
@@ -225,12 +258,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -545,21 +579,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA0E61E-2377-449A-AAC2-C63AB7E13499}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
     <col min="4" max="4" width="55.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -573,7 +607,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -585,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -597,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -609,7 +643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -621,7 +655,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -633,7 +667,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -643,7 +677,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -655,7 +689,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -667,7 +701,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -677,7 +711,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -687,7 +721,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -699,7 +733,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -711,7 +745,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
@@ -723,7 +757,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>35</v>
       </c>
@@ -735,7 +769,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>39</v>
       </c>
@@ -745,12 +779,53 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>